<commit_message>
Remove isolation and workflow test classes
</commit_message>
<xml_diff>
--- a/ismd-backend-validator/src/test/resources/com/dia/canonical/complete/testExcelProject.xlsx
+++ b/ismd-backend-validator/src/test/resources/com/dia/canonical/complete/testExcelProject.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardkoubek/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2AEB9A-043F-5F40-8691-4BB9DD981D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E2C687-0B53-5640-924A-4ADC7475D091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -294,18 +294,12 @@
     <t>Směrnice EU</t>
   </si>
   <si>
-    <t>https://ofn.gov.cz/slovn%C3%ADky/draft2/cs/#360-2023</t>
-  </si>
-  <si>
     <t>Datum</t>
   </si>
   <si>
     <t>Rodné číslo držitele řidičského průkazu subclass</t>
   </si>
   <si>
-    <t>Směrnice EU;https://ofn.gov.cz/slovn%C3%ADky/draft2/cs/#360-2023</t>
-  </si>
-  <si>
     <t>Název obecního úřadu obce s rozšířenou působností</t>
   </si>
   <si>
@@ -547,6 +541,12 @@
   </si>
   <si>
     <t>https://data.dia.gov.cz/příkladový-slovník-z-metodiky-popisu-dat/pojem/název-obecního-úřadu-obce-s-rozšířenou-působností-copy</t>
+  </si>
+  <si>
+    <t>https://ofn.gov.cz/slovníky/draft2/cs/#360-2023</t>
+  </si>
+  <si>
+    <t>Směrnice EU;https://ofn.gov.cz/slovníky/draft2/cs/#360-2023</t>
   </si>
 </sst>
 </file>
@@ -654,11 +654,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -992,7 +992,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G1" s="8"/>
     </row>
@@ -1053,23 +1053,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10" t="s">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="10"/>
+      <c r="L1" s="11"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1274,7 +1274,7 @@
     </row>
     <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="J10" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1314,10 +1314,10 @@
   <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1342,13 +1342,13 @@
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
       <c r="L1" t="s">
         <v>7</v>
       </c>
@@ -1484,24 +1484,24 @@
       <c r="E5" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>82</v>
+      <c r="F5" s="10" t="s">
+        <v>165</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="6"/>
       <c r="F6" t="s">
-        <v>85</v>
+        <v>166</v>
       </c>
       <c r="G6" t="s">
         <v>80</v>
@@ -1510,19 +1510,19 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
         <v>48</v>
       </c>
       <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="E7" t="s">
-        <v>88</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>89</v>
       </c>
       <c r="K7" t="s">
         <v>79</v>
@@ -1536,22 +1536,22 @@
     </row>
     <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>48</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>166</v>
+        <v>86</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>164</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="L8" s="8" t="s">
         <v>73</v>
@@ -1562,112 +1562,112 @@
     </row>
     <row r="9" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C9"/>
       <c r="K9" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="P9" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="O9" s="8" t="s">
+      <c r="Q9" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="P9" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q9" s="8" t="s">
-        <v>97</v>
-      </c>
       <c r="S9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B10" t="s">
         <v>35</v>
       </c>
       <c r="C10"/>
       <c r="K10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="N10" s="7" t="s">
         <v>38</v>
       </c>
       <c r="P10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Q10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B11" t="s">
         <v>35</v>
       </c>
       <c r="C11"/>
       <c r="K11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="P11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B12" t="s">
         <v>35</v>
       </c>
       <c r="C12"/>
       <c r="K12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s">
         <v>35</v>
       </c>
       <c r="C13"/>
       <c r="K13" t="s">
+        <v>106</v>
+      </c>
+      <c r="P13" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q13" t="s">
         <v>108</v>
-      </c>
-      <c r="P13" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B14" t="s">
         <v>35</v>
       </c>
       <c r="C14"/>
       <c r="K14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B15" t="s">
         <v>35</v>
@@ -1677,267 +1677,267 @@
         <v>79</v>
       </c>
       <c r="O15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B16" t="s">
         <v>35</v>
       </c>
       <c r="C16"/>
       <c r="K16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O16" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B17" t="s">
         <v>35</v>
       </c>
       <c r="K17" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="O17" t="s">
+        <v>93</v>
+      </c>
+      <c r="P17" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q17" t="s">
         <v>95</v>
-      </c>
-      <c r="P17" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B18" t="s">
         <v>35</v>
       </c>
       <c r="K18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N18" s="7" t="s">
         <v>38</v>
       </c>
       <c r="P18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Q18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B19" t="s">
         <v>35</v>
       </c>
       <c r="K19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="P19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B20" t="s">
         <v>35</v>
       </c>
       <c r="K20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="P20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B21" t="s">
         <v>35</v>
       </c>
       <c r="K21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="P21" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="Q21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B22" t="s">
         <v>35</v>
       </c>
       <c r="K22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B23" t="s">
         <v>35</v>
       </c>
       <c r="K23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="O23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B24" t="s">
         <v>35</v>
       </c>
       <c r="K24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="O24" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B25" t="s">
         <v>35</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="O25" t="s">
+        <v>93</v>
+      </c>
+      <c r="P25" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q25" t="s">
         <v>95</v>
-      </c>
-      <c r="P25" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
         <v>35</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="P26" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Q26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B27" t="s">
         <v>35</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="P27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B28" t="s">
         <v>35</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B29" t="s">
         <v>35</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="P29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="Q29" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B30" t="s">
         <v>35</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B31" t="s">
         <v>35</v>
       </c>
       <c r="K31" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="O31" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="O32" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1991,7 +1991,7 @@
     <hyperlink ref="N3" r:id="rId6" xr:uid="{0077AC49-67FF-4F2E-AA6F-EAB759D3B9DE}"/>
     <hyperlink ref="E4" r:id="rId7" xr:uid="{F0716393-D411-449F-B978-C2300959846E}"/>
     <hyperlink ref="N4" r:id="rId8" xr:uid="{A9858E43-03DA-490E-92BE-03AF2A29F5A2}"/>
-    <hyperlink ref="F5" r:id="rId9" location="360-2023" xr:uid="{F20AC61F-36F7-4689-9355-519256862D4D}"/>
+    <hyperlink ref="F5" r:id="rId9" location="360-2023" display="https://ofn.gov.cz/slovn%C3%ADky/draft2/cs/#360-2023" xr:uid="{F20AC61F-36F7-4689-9355-519256862D4D}"/>
     <hyperlink ref="N10" r:id="rId10" xr:uid="{40F63606-535C-49DB-B459-5A7AA75D96CE}"/>
     <hyperlink ref="N18" r:id="rId11" xr:uid="{C24AC8A4-40C2-4F40-9C4F-9EE7045F7F5C}"/>
     <hyperlink ref="K25" r:id="rId12" location="boolean" xr:uid="{E5D1CA02-0AF9-48C9-9B19-C90CF16900D0}"/>
@@ -2048,23 +2048,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="10" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10" t="s">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -2115,13 +2115,13 @@
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
         <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E3" t="s">
         <v>31</v>
@@ -2130,7 +2130,7 @@
         <v>32</v>
       </c>
       <c r="K3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -2138,20 +2138,20 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C4" t="s">
         <v>41</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F4" t="s">
         <v>24</v>
       </c>
       <c r="K4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -2159,22 +2159,22 @@
         <v>48</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>158</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>50</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -2182,19 +2182,19 @@
         <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C6" t="s">
         <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -2255,6 +2255,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="295d819b-bf18-46bf-9ff7-08a644d34552">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101003DFD27000E83C74CB14A0377F78F61D5" ma:contentTypeVersion="10" ma:contentTypeDescription="Vytvoří nový dokument" ma:contentTypeScope="" ma:versionID="f13eed8d3541cb6b85fe1ddbd6d3e5a1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="295d819b-bf18-46bf-9ff7-08a644d34552" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8ad5fcc376830e9bb44e0d894e82739e" ns2:_="">
     <xsd:import namespace="295d819b-bf18-46bf-9ff7-08a644d34552"/>
@@ -2432,26 +2451,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A057CC-F79E-47F3-98AA-B167136EC5C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="295d819b-bf18-46bf-9ff7-08a644d34552"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="295d819b-bf18-46bf-9ff7-08a644d34552">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82936FB6-BA39-4A9D-9D90-41D252778FFD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A548783-F638-4AE1-812F-39BB704400B6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2467,22 +2485,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82936FB6-BA39-4A9D-9D90-41D252778FFD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A057CC-F79E-47F3-98AA-B167136EC5C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="295d819b-bf18-46bf-9ff7-08a644d34552"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
excel reader clean up, hierarchy processing
</commit_message>
<xml_diff>
--- a/ismd-backend-validator/src/test/resources/com/dia/canonical/complete/testExcelProject.xlsx
+++ b/ismd-backend-validator/src/test/resources/com/dia/canonical/complete/testExcelProject.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardkoubek/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E2C687-0B53-5640-924A-4ADC7475D091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{88798B99-CDDA-484F-A5D9-4197F4A0EFC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19960" firstSheet="3" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slovník" sheetId="6" r:id="rId1"/>
@@ -38,6 +38,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -46,11 +47,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="167">
   <si>
     <t>Název slovníku:</t>
   </si>
   <si>
+    <t>Slovník dle metodiky dat Digitální a informační agentury</t>
+  </si>
+  <si>
     <t>Popis slovníku:</t>
   </si>
   <si>
@@ -222,6 +226,9 @@
     <t>https://slovník.gov.cz/legislativní/sbírka/111/2009/pojem/adresa</t>
   </si>
   <si>
+    <t>očekávané, cizí pojem</t>
+  </si>
+  <si>
     <t>Charakteristiky vyhlášky 360/2023</t>
   </si>
   <si>
@@ -294,12 +301,18 @@
     <t>Směrnice EU</t>
   </si>
   <si>
+    <t>https://ofn.gov.cz/slovníky/draft2/cs/#360-2023</t>
+  </si>
+  <si>
     <t>Datum</t>
   </si>
   <si>
     <t>Rodné číslo držitele řidičského průkazu subclass</t>
   </si>
   <si>
+    <t>Směrnice EU;https://ofn.gov.cz/slovníky/draft2/cs/#360-2023</t>
+  </si>
+  <si>
     <t>Název obecního úřadu obce s rozšířenou působností</t>
   </si>
   <si>
@@ -318,6 +331,9 @@
     <t>Řidičský průkaz obsahuje název úřadu, který řidičský průkaz vydal (což je vždy obecní úřad obce s rozšířenou působností).</t>
   </si>
   <si>
+    <t>https://data.dia.gov.cz/příkladový-slovník-z-metodiky-popisu-dat/pojem/název-obecního-úřadu-obce-s-rozšířenou-působností-copy</t>
+  </si>
+  <si>
     <t>test - má být literal</t>
   </si>
   <si>
@@ -336,6 +352,9 @@
     <t>Identifikační</t>
   </si>
   <si>
+    <t>resolved</t>
+  </si>
+  <si>
     <t>Věk na ŘP S</t>
   </si>
   <si>
@@ -529,31 +548,13 @@
   </si>
   <si>
     <t>https://data.dia.gov.cz/příkladový-slovník-z-metodiky-popisu-dat/pojem/sídlí-na-adrese</t>
-  </si>
-  <si>
-    <t>Slovník dle metodiky dat Digitální a informační agentury</t>
-  </si>
-  <si>
-    <t>resolved</t>
-  </si>
-  <si>
-    <t>očekávané, cizí pojem</t>
-  </si>
-  <si>
-    <t>https://data.dia.gov.cz/příkladový-slovník-z-metodiky-popisu-dat/pojem/název-obecního-úřadu-obce-s-rozšířenou-působností-copy</t>
-  </si>
-  <si>
-    <t>https://ofn.gov.cz/slovníky/draft2/cs/#360-2023</t>
-  </si>
-  <si>
-    <t>Směrnice EU;https://ofn.gov.cz/slovníky/draft2/cs/#360-2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -609,6 +610,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -637,7 +644,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -651,19 +658,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{31B833F2-3BD0-4DAC-BB9E-D63D96AAF249}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Správně" xfId="2" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -978,39 +984,39 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="59" customWidth="1"/>
-    <col min="2" max="2" width="75.6640625" customWidth="1"/>
+    <col min="2" max="2" width="75.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15.95">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>161</v>
+        <v>1</v>
       </c>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15.95">
       <c r="A2" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15.95">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G3" s="8"/>
     </row>
@@ -1031,198 +1037,198 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" customWidth="1"/>
+    <col min="1" max="1" width="41.28515625" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.5" customWidth="1"/>
-    <col min="5" max="5" width="100.83203125" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="9" width="15.33203125" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" customWidth="1"/>
-    <col min="12" max="12" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" customWidth="1"/>
+    <col min="5" max="5" width="100.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11" t="s">
+    <row r="1" spans="1:12">
+      <c r="B1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="11"/>
-    </row>
-    <row r="2" spans="1:12" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="13"/>
+    </row>
+    <row r="2" spans="1:12" s="3" customFormat="1" ht="32.1">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.95">
       <c r="A3" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.95">
+      <c r="A4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="C4"/>
       <c r="D4" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L4" s="8">
         <v>1234</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="15.95">
       <c r="A5" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C5"/>
       <c r="D5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.95">
+      <c r="A6" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="C6"/>
       <c r="D6" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.95">
       <c r="A7" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7"/>
       <c r="D7" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K7" s="8">
         <v>998</v>
@@ -1231,50 +1237,50 @@
         <v>998</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="15.95">
       <c r="A8" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="8" customFormat="1" ht="15.95">
       <c r="A9" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.95">
       <c r="J10" s="8" t="s">
-        <v>163</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1314,634 +1320,634 @@
   <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="P9" sqref="P9"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.5" customWidth="1"/>
-    <col min="5" max="5" width="60.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="9" width="15.33203125" customWidth="1"/>
-    <col min="11" max="11" width="16.5" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" customWidth="1"/>
-    <col min="14" max="14" width="21.5" customWidth="1"/>
-    <col min="15" max="15" width="13.5" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" customWidth="1"/>
-    <col min="17" max="17" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" customWidth="1"/>
+    <col min="5" max="5" width="60.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="9" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="16" max="16" width="25.5703125" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="15.95">
       <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
+      <c r="F1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
       <c r="L1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" s="3" customFormat="1" ht="29.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="3" customFormat="1" ht="29.85" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.75">
       <c r="A3" s="8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15.95">
+      <c r="A4" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="K3" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="N3" s="8" t="s">
+      <c r="H4" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="M4" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="H4" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="J4" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:19" ht="15.95">
       <c r="A5" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" s="6"/>
       <c r="E5" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>165</v>
+        <v>83</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" s="6"/>
       <c r="F6" t="s">
-        <v>166</v>
+        <v>87</v>
       </c>
       <c r="G6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E7" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="K7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15.95">
       <c r="A8" s="8" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>164</v>
+        <v>90</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15.75">
       <c r="A9" s="8" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9"/>
       <c r="K9" s="8" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="O9" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="P9" s="9" t="s">
-        <v>94</v>
+        <v>98</v>
+      </c>
+      <c r="P9" s="12" t="s">
+        <v>99</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="S9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10"/>
       <c r="K10" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P10" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="Q10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11"/>
       <c r="K11" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="P11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12"/>
       <c r="K12" t="s">
-        <v>82</v>
-      </c>
-      <c r="P12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="O12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C13"/>
       <c r="K13" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="P13" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="Q13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14"/>
       <c r="K14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C15"/>
       <c r="K15" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="O15" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16"/>
       <c r="K16" t="s">
+        <v>120</v>
+      </c>
+      <c r="O16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" t="s">
+        <v>123</v>
+      </c>
+      <c r="O17" t="s">
+        <v>98</v>
+      </c>
+      <c r="P17" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K18" t="s">
+        <v>125</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="P18" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K19" t="s">
+        <v>127</v>
+      </c>
+      <c r="P19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="K20" t="s">
+        <v>129</v>
+      </c>
+      <c r="O20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="K21" t="s">
+        <v>131</v>
+      </c>
+      <c r="P21" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q21" t="s">
         <v>114</v>
       </c>
-      <c r="O16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>116</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="K17" t="s">
-        <v>117</v>
-      </c>
-      <c r="O17" t="s">
-        <v>93</v>
-      </c>
-      <c r="P17" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" t="s">
+        <v>132</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="K22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="K23" t="s">
+        <v>135</v>
+      </c>
+      <c r="O23" t="s">
         <v>118</v>
       </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="K18" t="s">
-        <v>119</v>
-      </c>
-      <c r="N18" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="P18" t="s">
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="K24" t="s">
+        <v>137</v>
+      </c>
+      <c r="O24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="O25" t="s">
         <v>98</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="P25" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>120</v>
-      </c>
-      <c r="B19" t="s">
-        <v>35</v>
-      </c>
-      <c r="K19" t="s">
+      <c r="Q25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" t="s">
+        <v>140</v>
+      </c>
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="P26" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="P27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="O28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" t="s">
+        <v>146</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="P29" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30" t="s">
+        <v>148</v>
+      </c>
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31" t="s">
+        <v>150</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="O31" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="A32" t="s">
+        <v>152</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="O32" t="s">
         <v>121</v>
       </c>
-      <c r="P19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>122</v>
-      </c>
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="K20" t="s">
-        <v>123</v>
-      </c>
-      <c r="P20" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>124</v>
-      </c>
-      <c r="B21" t="s">
-        <v>35</v>
-      </c>
-      <c r="K21" t="s">
-        <v>125</v>
-      </c>
-      <c r="P21" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>126</v>
-      </c>
-      <c r="B22" t="s">
-        <v>35</v>
-      </c>
-      <c r="K22" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>128</v>
-      </c>
-      <c r="B23" t="s">
-        <v>35</v>
-      </c>
-      <c r="K23" t="s">
-        <v>129</v>
-      </c>
-      <c r="O23" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>130</v>
-      </c>
-      <c r="B24" t="s">
-        <v>35</v>
-      </c>
-      <c r="K24" t="s">
-        <v>131</v>
-      </c>
-      <c r="O24" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>132</v>
-      </c>
-      <c r="B25" t="s">
-        <v>35</v>
-      </c>
-      <c r="K25" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="O25" t="s">
-        <v>93</v>
-      </c>
-      <c r="P25" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>134</v>
-      </c>
-      <c r="B26" t="s">
-        <v>35</v>
-      </c>
-      <c r="K26" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="P26" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>136</v>
-      </c>
-      <c r="B27" t="s">
-        <v>35</v>
-      </c>
-      <c r="K27" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="P27" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>138</v>
-      </c>
-      <c r="B28" t="s">
-        <v>35</v>
-      </c>
-      <c r="K28" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="P28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>140</v>
-      </c>
-      <c r="B29" t="s">
-        <v>35</v>
-      </c>
-      <c r="K29" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="P29" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>142</v>
-      </c>
-      <c r="B30" t="s">
-        <v>35</v>
-      </c>
-      <c r="K30" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>144</v>
-      </c>
-      <c r="B31" t="s">
-        <v>35</v>
-      </c>
-      <c r="K31" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="O31" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>146</v>
-      </c>
-      <c r="B32" t="s">
-        <v>35</v>
-      </c>
-      <c r="K32" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="O32" t="s">
-        <v>115</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:N2" xr:uid="{13DDA33D-1F62-45BA-B8E5-510B45B31189}"/>
+  <autoFilter ref="A2:N32" xr:uid="{13DDA33D-1F62-45BA-B8E5-510B45B31189}"/>
   <dataConsolidate/>
   <mergeCells count="1">
     <mergeCell ref="F1:J1"/>
@@ -1969,13 +1975,13 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Nápověda" prompt="Zdroj, který nedefinuje, nýbrž upřesňuje význam pojmu." sqref="F3:F1048576" xr:uid="{EB79E25D-54BE-4B15-9A1F-25ADADD23270}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Nápověda" prompt="Další, neoficiální název pojmu." sqref="H3:H1048576" xr:uid="{B93F9303-0069-48FD-B2F9-165E1F031165}"/>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="A2:XFD2 P9" xr:uid="{B9B6ABAB-E396-4C2A-ACC5-4C9426BE2CE8}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:P8 P10:P1048576" xr:uid="{BD85CD45-49CC-44E4-A936-E7668DF670F4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:P8 O12 P10:P11 O20 P13:P19 O28 P21:P27 P29:P1048576" xr:uid="{BD85CD45-49CC-44E4-A936-E7668DF670F4}">
       <formula1>"Základních registrů,Jiných agend,Vlastní,Provozní"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Nápověda" prompt="Přiřazení do kategorie, která charakterizuje odpovídající údaj z hlediska způsobu jeho získání či vzniku v rámci dané věcné oblasti." sqref="O3:O1048576" xr:uid="{20C3A296-E413-4528-88FE-0B2E97CF88B5}">
       <formula1>"Základních registrů,Jiných agend,Vlastní,Provozní"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Nápověda" prompt="Přiřazení do kategorie, která charakterizuje odpovídající údaj z hlediska způsobu jeho sdílení mimo danou věcnou oblast, ve které je spravován." sqref="P3:P8 P10:P1048576" xr:uid="{EE081268-BA8A-4E41-9667-C403DCE905B7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Nápověda" prompt="Přiřazení do kategorie, která charakterizuje odpovídající údaj z hlediska způsobu jeho sdílení mimo danou věcnou oblast, ve které je spravován." sqref="P3:P8 O12 P10:P11 O20 P13:P19 O28 P21:P27 P29:P1048576" xr:uid="{EE081268-BA8A-4E41-9667-C403DCE905B7}">
       <formula1>"Veřejně přístupné,Poskytované na žádost,Zpřístupňované pro výkon agendy,Nesdílené"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Nápověda" prompt="Přiřazení do kategorie, která charakterizuje odpovídající údaj z hlediska toho, nakolik je jeho obsah spojitelný s konkrétním identifikovatelným subjektem práva." sqref="Q3:Q1048576" xr:uid="{32323A13-298D-48DC-A07F-56D048A970BA}">
@@ -2022,185 +2028,251 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E5F5C28-51A8-4892-87C1-7E525C9ADAB6}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="Q7" sqref="Q7"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
-    <col min="4" max="4" width="38.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="37.5" customWidth="1"/>
-    <col min="6" max="6" width="60.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" customWidth="1"/>
-    <col min="9" max="10" width="15.33203125" customWidth="1"/>
-    <col min="12" max="12" width="23.6640625" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" customWidth="1"/>
-    <col min="14" max="14" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" customWidth="1"/>
+    <col min="6" max="6" width="60.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+    <col min="9" max="10" width="15.28515625" customWidth="1"/>
+    <col min="12" max="12" width="23.7109375" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" customWidth="1"/>
+    <col min="14" max="14" width="21.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D1" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="11" t="s">
+    <row r="1" spans="1:17">
+      <c r="D1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-    </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="3" customFormat="1" ht="45.75">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="30.75">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="L3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M3" t="s">
+        <v>76</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="O3" t="s">
+        <v>121</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="30.75">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+      <c r="L4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M4" t="s">
+        <v>75</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="30.75">
       <c r="A5" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+      <c r="O5" t="s">
+        <v>98</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q5" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="F6" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="K6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+      <c r="L6" t="s">
+        <v>75</v>
+      </c>
+      <c r="O6" t="s">
+        <v>118</v>
+      </c>
+      <c r="P6" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17">
       <c r="D8"/>
     </row>
   </sheetData>
@@ -2229,10 +2301,13 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Nápověda" prompt="Vložte odkaz na zdroj definice - Zákony pro lidi/eSbírka/dokument... U odkazu na web zajistěte, že je odkaz co nejkonkrétnější, tj. že odkazuje na konkrétní paragraf/písmeno a ne na celý zákon." sqref="F6:F1048576 F3:F4" xr:uid="{4A24DBC4-BDC9-40BF-B16C-243A42680C2F}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Nápověda" prompt="Další, neoficiální název pojmu." sqref="I3:I1048576" xr:uid="{C3DF9CEE-9484-4F47-81FC-56D042A703C5}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Nápověda" prompt="Zdroj, který nedefinuje, nýbrž upřesňuje význam pojmu." sqref="G3:G1048576" xr:uid="{38C3392C-BFC6-4684-9E00-2EDEA32BA6E3}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="A2:N2 R2:XFD2" xr:uid="{28F27C0A-59BA-4456-ADB9-FB5F5D1BCD11}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="A2:XFD2" xr:uid="{28F27C0A-59BA-4456-ADB9-FB5F5D1BCD11}"/>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="N3" r:id="rId1" xr:uid="{DAF1F0F9-F625-466C-9FDF-F33523E5DC30}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -2265,15 +2340,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101003DFD27000E83C74CB14A0377F78F61D5" ma:contentTypeVersion="10" ma:contentTypeDescription="Vytvoří nový dokument" ma:contentTypeScope="" ma:versionID="f13eed8d3541cb6b85fe1ddbd6d3e5a1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="295d819b-bf18-46bf-9ff7-08a644d34552" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8ad5fcc376830e9bb44e0d894e82739e" ns2:_="">
     <xsd:import namespace="295d819b-bf18-46bf-9ff7-08a644d34552"/>
@@ -2451,38 +2517,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A057CC-F79E-47F3-98AA-B167136EC5C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="295d819b-bf18-46bf-9ff7-08a644d34552"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A057CC-F79E-47F3-98AA-B167136EC5C6}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82936FB6-BA39-4A9D-9D90-41D252778FFD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A548783-F638-4AE1-812F-39BB704400B6}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A548783-F638-4AE1-812F-39BB704400B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="295d819b-bf18-46bf-9ff7-08a644d34552"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82936FB6-BA39-4A9D-9D90-41D252778FFD}"/>
 </file>
</xml_diff>